<commit_message>
sorted countries by key
</commit_message>
<xml_diff>
--- a/dataDir/models/WarehouseConfig.xlsx
+++ b/dataDir/models/WarehouseConfig.xlsx
@@ -123,7 +123,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -438,7 +438,7 @@
     <col min="3" max="3" style="2" width="65.14785714285713" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -449,7 +449,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -460,7 +460,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -471,7 +471,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -482,7 +482,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -493,7 +493,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>

</xml_diff>